<commit_message>
Data V3.0. Add code for creating districts of parks.
</commit_message>
<xml_diff>
--- a/data/table.xlsx
+++ b/data/table.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WarsawParkInfo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFEA4BD-B308-4914-B825-B3C340111925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3079C9EE-A0FF-4673-9FF5-44B4EE10FC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Park" sheetId="1" r:id="rId1"/>
     <sheet name="District" sheetId="2" r:id="rId2"/>
+    <sheet name="District_of_park" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="290">
   <si>
     <t>park_name</t>
   </si>
@@ -874,9 +875,6 @@
   </si>
   <si>
     <t>pomiędzy ul. Powsińską, Okrężną i Klarysewska Wejście od strony ul. Powsińskiej i Klarysewskiej</t>
-  </si>
-  <si>
-    <t>Mokotowa, Ochoty i Śródmieścia</t>
   </si>
   <si>
     <t>w obrębie ulic Żwirki i Wigury, Rostafińskich, Rokitnickiej, Batorego oraz Al. Niepodległości</t>
@@ -930,7 +928,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -943,14 +941,8 @@
         <bgColor rgb="FFC0504D"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2DCDB"/>
-        <bgColor rgb="FFF2DCDB"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1085,105 +1077,17 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1220,33 +1124,323 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="22">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1331,214 +1525,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1553,38 +1539,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CC73D255-BFDD-4166-B89D-0F3CF8BA4C28}" name="Table2" displayName="Table2" ref="A1:G73" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="A1:G73" xr:uid="{CC73D255-BFDD-4166-B89D-0F3CF8BA4C28}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CC73D255-BFDD-4166-B89D-0F3CF8BA4C28}" name="Park" displayName="Park" ref="A1:F73" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:F73" xr:uid="{CC73D255-BFDD-4166-B89D-0F3CF8BA4C28}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C93E0E94-FC0C-4B53-B13D-547DBC6D2545}" name="park_id" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{F9C0D35C-5463-49C1-A53C-D6794E6814B2}" name="park_name" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{F2ADA958-3D05-4FA2-B7CB-0EF569759435}" name="attractions" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{046A015F-409D-4F6E-B7C8-6E3EF0691271}" name="area" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{FE8DE984-7D08-4E87-879D-826DCF23AF47}" name="position" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{999B4A05-4F51-4EC1-A42E-C4255BC12159}" name="district_id" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{59FB128A-F489-490B-BF9F-E2755F00D769}" name="rating" dataDxfId="6"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{C93E0E94-FC0C-4B53-B13D-547DBC6D2545}" name="park_id" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F9C0D35C-5463-49C1-A53C-D6794E6814B2}" name="park_name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{F2ADA958-3D05-4FA2-B7CB-0EF569759435}" name="attractions" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{046A015F-409D-4F6E-B7C8-6E3EF0691271}" name="area" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{FE8DE984-7D08-4E87-879D-826DCF23AF47}" name="position" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{59FB128A-F489-490B-BF9F-E2755F00D769}" name="rating" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EDABDA9C-3963-41AC-BCC5-CDB447D89752}" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EDABDA9C-3963-41AC-BCC5-CDB447D89752}" name="District" displayName="District" ref="A1:B19" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
   <autoFilter ref="A1:B19" xr:uid="{EDABDA9C-3963-41AC-BCC5-CDB447D89752}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EC0619C8-5060-464F-803E-3C572E2E48BE}" name="district_id" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{35E8DD57-4ACF-48B4-AE16-9423FF4D41BE}" name="Dzielnica" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{EC0619C8-5060-464F-803E-3C572E2E48BE}" name="district_id" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{35E8DD57-4ACF-48B4-AE16-9423FF4D41BE}" name="Dzielnica" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{47540FD9-ABFA-4064-ADAB-F1249077C742}" name="District_of_park" displayName="District_of_park" ref="A1:B75" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:B75" xr:uid="{47540FD9-ABFA-4064-ADAB-F1249077C742}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FD34BC55-7544-491B-A184-05BFFD619DF3}" name="district_id" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{694B2DA6-6F68-4693-A24F-0130116F9F0E}" name="park_id" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1875,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1886,34 +1884,32 @@
     <col min="1" max="1" width="10.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="6" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
+      <c r="F1" s="25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1925,16 +1921,15 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="23"/>
-    </row>
-    <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19">
+      <c r="F2" s="14">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1946,16 +1941,15 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1">
-        <v>8</v>
-      </c>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
+      <c r="F3" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1967,16 +1961,15 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1">
-        <v>8</v>
-      </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
+      <c r="F4" s="14">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1988,16 +1981,15 @@
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
+      <c r="F5" s="14">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -2009,16 +2001,15 @@
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
+      <c r="F6" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2033,13 +2024,12 @@
       <c r="E7" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="F7" s="1">
-        <v>13</v>
-      </c>
-      <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+      <c r="F7" s="14">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -2051,16 +2041,15 @@
       <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="1">
-        <v>10</v>
-      </c>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
+      <c r="F8" s="14">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2072,16 +2061,15 @@
       <c r="D9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+      <c r="F9" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -2093,16 +2081,15 @@
       <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F10" s="1">
-        <v>8</v>
-      </c>
-      <c r="G10" s="14"/>
-    </row>
-    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+      <c r="F10" s="14">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2114,16 +2101,15 @@
       <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="1">
-        <v>3</v>
-      </c>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+      <c r="F11" s="14">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2135,16 +2121,15 @@
       <c r="D12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="1">
-        <v>8</v>
-      </c>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
+      <c r="F12" s="14">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2156,16 +2141,15 @@
       <c r="D13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F13" s="1">
-        <v>12</v>
-      </c>
-      <c r="G13" s="15"/>
-    </row>
-    <row r="14" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19">
+      <c r="F13" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2177,16 +2161,15 @@
       <c r="D14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19">
+      <c r="F14" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2198,16 +2181,15 @@
       <c r="D15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="1">
-        <v>8</v>
-      </c>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
+      <c r="F15" s="14">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -2219,16 +2201,15 @@
       <c r="D16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="1">
-        <v>11</v>
-      </c>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19">
+      <c r="F16" s="14">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2240,16 +2221,15 @@
       <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="1">
-        <v>11</v>
-      </c>
-      <c r="G17" s="15"/>
-    </row>
-    <row r="18" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19">
+      <c r="F17" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2261,16 +2241,15 @@
       <c r="D18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="1">
-        <v>15</v>
-      </c>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19">
+      <c r="F18" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -2282,16 +2261,13 @@
       <c r="D19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F19" s="1">
-        <v>15</v>
-      </c>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19">
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -2303,16 +2279,13 @@
       <c r="D20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="1">
-        <v>5</v>
-      </c>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19">
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -2324,16 +2297,13 @@
       <c r="D21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19">
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -2345,16 +2315,13 @@
       <c r="D22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19">
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -2366,16 +2333,13 @@
       <c r="D23" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="1">
-        <v>10</v>
-      </c>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -2387,16 +2351,13 @@
       <c r="D24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F24" s="1">
-        <v>6</v>
-      </c>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19">
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -2408,16 +2369,13 @@
       <c r="D25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F25" s="1">
-        <v>10</v>
-      </c>
-      <c r="G25" s="15"/>
-    </row>
-    <row r="26" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19">
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2429,16 +2387,13 @@
       <c r="D26" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F26" s="1">
-        <v>7</v>
-      </c>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19">
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2450,16 +2405,13 @@
       <c r="D27" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F27" s="1">
-        <v>7</v>
-      </c>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19">
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2471,16 +2423,13 @@
       <c r="D28" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F28" s="1">
-        <v>8</v>
-      </c>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19">
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2492,16 +2441,13 @@
       <c r="D29" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="1">
-        <v>2</v>
-      </c>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19">
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2513,16 +2459,13 @@
       <c r="D30" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F30" s="1">
-        <v>4</v>
-      </c>
-      <c r="G30" s="14"/>
-    </row>
-    <row r="31" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19">
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2532,16 +2475,13 @@
       <c r="D31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="G31" s="15"/>
-    </row>
-    <row r="32" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19">
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2553,16 +2493,13 @@
       <c r="D32" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F32" s="1">
-        <v>8</v>
-      </c>
-      <c r="G32" s="14"/>
-    </row>
-    <row r="33" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="19">
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2574,16 +2511,13 @@
       <c r="D33" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F33" s="1">
-        <v>8</v>
-      </c>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="19">
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14">
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2595,16 +2529,13 @@
       <c r="D34" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F34" s="1">
-        <v>6</v>
-      </c>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19">
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2616,16 +2547,13 @@
       <c r="D35" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="F35" s="1">
-        <v>5</v>
-      </c>
-      <c r="G35" s="15"/>
-    </row>
-    <row r="36" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="19">
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
         <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2635,16 +2563,13 @@
       <c r="D36" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="19">
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2656,16 +2581,13 @@
       <c r="D37" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F37" s="1">
-        <v>1</v>
-      </c>
-      <c r="G37" s="15"/>
-    </row>
-    <row r="38" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="19">
+      <c r="F37" s="14"/>
+    </row>
+    <row r="38" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14">
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2677,16 +2599,13 @@
       <c r="D38" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-      <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="19">
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="14">
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2698,16 +2617,13 @@
       <c r="D39" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F39" s="1">
-        <v>13</v>
-      </c>
-      <c r="G39" s="15"/>
-    </row>
-    <row r="40" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19">
+      <c r="F39" s="14"/>
+    </row>
+    <row r="40" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14">
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2719,16 +2635,13 @@
       <c r="D40" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F40" s="1">
-        <v>13</v>
-      </c>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19">
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14">
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2740,16 +2653,13 @@
       <c r="D41" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="F41" s="1">
-        <v>13</v>
-      </c>
-      <c r="G41" s="15"/>
-    </row>
-    <row r="42" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19">
+      <c r="F41" s="14"/>
+    </row>
+    <row r="42" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14">
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2761,16 +2671,13 @@
       <c r="D42" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F42" s="1">
-        <v>3</v>
-      </c>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="19">
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14">
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2782,16 +2689,13 @@
       <c r="D43" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F43" s="1">
-        <v>3</v>
-      </c>
-      <c r="G43" s="15"/>
-    </row>
-    <row r="44" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="19">
+      <c r="F43" s="14"/>
+    </row>
+    <row r="44" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14">
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2803,16 +2707,13 @@
       <c r="D44" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F44" s="1">
-        <v>8</v>
-      </c>
-      <c r="G44" s="14"/>
-    </row>
-    <row r="45" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19">
+      <c r="F44" s="14"/>
+    </row>
+    <row r="45" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="14">
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -2824,16 +2725,13 @@
       <c r="D45" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F45" s="1">
-        <v>10</v>
-      </c>
-      <c r="G45" s="15"/>
-    </row>
-    <row r="46" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19">
+      <c r="F45" s="14"/>
+    </row>
+    <row r="46" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="14">
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2843,16 +2741,13 @@
       <c r="D46" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F46" s="1">
-        <v>10</v>
-      </c>
-      <c r="G46" s="14"/>
-    </row>
-    <row r="47" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="19">
+      <c r="F46" s="14"/>
+    </row>
+    <row r="47" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="14">
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -2864,16 +2759,13 @@
       <c r="D47" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F47" s="1">
-        <v>10</v>
-      </c>
-      <c r="G47" s="15"/>
-    </row>
-    <row r="48" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="19">
+      <c r="F47" s="14"/>
+    </row>
+    <row r="48" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="14">
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -2885,16 +2777,13 @@
       <c r="D48" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F48" s="1">
-        <v>4</v>
-      </c>
-      <c r="G48" s="14"/>
-    </row>
-    <row r="49" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="19">
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="14">
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -2906,16 +2795,13 @@
       <c r="D49" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F49" s="1">
-        <v>5</v>
-      </c>
-      <c r="G49" s="15"/>
-    </row>
-    <row r="50" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="19">
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14">
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -2927,16 +2813,13 @@
       <c r="D50" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F50" s="1">
-        <v>5</v>
-      </c>
-      <c r="G50" s="14"/>
-    </row>
-    <row r="51" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="19">
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="14">
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -2946,16 +2829,13 @@
       <c r="D51" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F51" s="1">
-        <v>15</v>
-      </c>
-      <c r="G51" s="15"/>
-    </row>
-    <row r="52" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="19">
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="14">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -2967,16 +2847,13 @@
       <c r="D52" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F52" s="1">
-        <v>5</v>
-      </c>
-      <c r="G52" s="14"/>
-    </row>
-    <row r="53" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="19">
+      <c r="F52" s="14"/>
+    </row>
+    <row r="53" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14">
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -2988,16 +2865,13 @@
       <c r="D53" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="F53" s="1">
-        <v>1</v>
-      </c>
-      <c r="G53" s="15"/>
-    </row>
-    <row r="54" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="19">
+      <c r="F53" s="14"/>
+    </row>
+    <row r="54" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="14">
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -3009,16 +2883,13 @@
       <c r="D54" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F54" s="1">
-        <v>1</v>
-      </c>
-      <c r="G54" s="14"/>
-    </row>
-    <row r="55" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="19">
+      <c r="F54" s="14"/>
+    </row>
+    <row r="55" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="14">
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -3028,16 +2899,13 @@
       <c r="D55" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="F55" s="1">
-        <v>4</v>
-      </c>
-      <c r="G55" s="15"/>
-    </row>
-    <row r="56" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="19">
+      <c r="F55" s="14"/>
+    </row>
+    <row r="56" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14">
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -3049,16 +2917,13 @@
       <c r="D56" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F56" s="1">
-        <v>1</v>
-      </c>
-      <c r="G56" s="14"/>
-    </row>
-    <row r="57" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="19">
+      <c r="F56" s="14"/>
+    </row>
+    <row r="57" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="14">
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -3070,16 +2935,13 @@
       <c r="D57" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F57" s="1" t="s">
+      <c r="E57" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G57" s="15"/>
-    </row>
-    <row r="58" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="19">
+      <c r="F57" s="14"/>
+    </row>
+    <row r="58" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="14">
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -3092,17 +2954,14 @@
         <v>211</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F58" s="1">
-        <v>0</v>
-      </c>
-      <c r="G58" s="14">
+        <v>285</v>
+      </c>
+      <c r="F58" s="14">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="19">
+    <row r="59" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="14">
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -3112,18 +2971,15 @@
       <c r="D59" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F59" s="1">
-        <v>10</v>
-      </c>
-      <c r="G59" s="15">
+      <c r="F59" s="14">
         <v>4.3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="19">
+    <row r="60" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="14">
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -3133,18 +2989,15 @@
       <c r="D60" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F60" s="1">
-        <v>2</v>
-      </c>
-      <c r="G60" s="14">
+      <c r="F60" s="14">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="19">
+    <row r="61" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="14">
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -3156,18 +3009,15 @@
       <c r="D61" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F61" s="1">
-        <v>8</v>
-      </c>
-      <c r="G61" s="15">
+      <c r="F61" s="14">
         <v>4.7</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="19">
+    <row r="62" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="14">
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -3177,18 +3027,15 @@
       <c r="D62" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F62" s="1">
-        <v>0</v>
-      </c>
-      <c r="G62" s="14">
+      <c r="F62" s="14">
         <v>4.7</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="19">
+    <row r="63" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="14">
         <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -3198,18 +3045,15 @@
       <c r="D63" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F63" s="1">
-        <v>5</v>
-      </c>
-      <c r="G63" s="15">
+      <c r="F63" s="14">
         <v>4.5</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="19">
+    <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="14">
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -3219,18 +3063,15 @@
       <c r="D64" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F64" s="1">
-        <v>0</v>
-      </c>
-      <c r="G64" s="14">
+      <c r="F64" s="14">
         <v>4.2</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="19">
+    <row r="65" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="14">
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -3240,18 +3081,15 @@
       <c r="D65" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F65" s="1">
-        <v>8</v>
-      </c>
-      <c r="G65" s="15">
+      <c r="F65" s="14">
         <v>4.5</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="19">
+    <row r="66" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="14">
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -3263,18 +3101,15 @@
       <c r="D66" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F66" s="1">
-        <v>5</v>
-      </c>
-      <c r="G66" s="14">
+      <c r="F66" s="14">
         <v>4.8</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="19">
+    <row r="67" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="14">
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
@@ -3284,18 +3119,15 @@
       <c r="D67" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F67" s="1">
-        <v>10</v>
-      </c>
-      <c r="G67" s="15">
+      <c r="E67" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F67" s="14">
         <v>4.5</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="19">
+    <row r="68" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="14">
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -3307,18 +3139,15 @@
       <c r="D68" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="F68" s="1">
-        <v>4</v>
-      </c>
-      <c r="G68" s="14">
+      <c r="E68" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="F68" s="14">
         <v>4.7</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="19">
+    <row r="69" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="14">
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -3330,18 +3159,15 @@
       <c r="D69" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="F69" s="1">
-        <v>4</v>
-      </c>
-      <c r="G69" s="15">
+      <c r="E69" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F69" s="14">
         <v>4.3</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="19">
+    <row r="70" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="14">
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -3353,18 +3179,15 @@
       <c r="D70" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="F70" s="1">
-        <v>1</v>
-      </c>
-      <c r="G70" s="14">
+      <c r="F70" s="14">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="19">
+    <row r="71" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="14">
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -3374,18 +3197,15 @@
       <c r="D71" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F71" s="1">
-        <v>8</v>
-      </c>
-      <c r="G71" s="15">
+      <c r="F71" s="14">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="19">
+    <row r="72" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="14">
         <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -3395,39 +3215,33 @@
       <c r="D72" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F72" s="1">
-        <v>8</v>
-      </c>
-      <c r="G72" s="14">
+      <c r="F72" s="14">
         <v>4.8</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="20">
+    <row r="73" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="18">
         <v>71</v>
       </c>
-      <c r="B73" s="21" t="s">
+      <c r="B73" s="26" t="s">
         <v>252</v>
       </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22" t="s">
+      <c r="C73" s="21"/>
+      <c r="D73" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="E73" s="22" t="s">
+      <c r="E73" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="F73" s="22">
-        <v>8</v>
-      </c>
-      <c r="G73" s="24">
+      <c r="F73" s="14">
         <v>4.5</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G74" s="13"/>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F74" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3442,7 +3256,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3609,4 +3423,625 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32577B8C-4529-4E21-9FCB-D712CEE7DBA7}">
+  <dimension ref="A1:B75"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>8</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>8</v>
+      </c>
+      <c r="B4" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>1</v>
+      </c>
+      <c r="B6" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>10</v>
+      </c>
+      <c r="B8" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>0</v>
+      </c>
+      <c r="B9" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>8</v>
+      </c>
+      <c r="B10" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>3</v>
+      </c>
+      <c r="B11" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>8</v>
+      </c>
+      <c r="B12" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>0</v>
+      </c>
+      <c r="B14" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>8</v>
+      </c>
+      <c r="B15" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>11</v>
+      </c>
+      <c r="B16" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>11</v>
+      </c>
+      <c r="B17" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>15</v>
+      </c>
+      <c r="B19" s="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <v>5</v>
+      </c>
+      <c r="B20" s="15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>0</v>
+      </c>
+      <c r="B21" s="15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
+        <v>0</v>
+      </c>
+      <c r="B22" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
+        <v>10</v>
+      </c>
+      <c r="B23" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>6</v>
+      </c>
+      <c r="B24" s="15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>10</v>
+      </c>
+      <c r="B25" s="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
+        <v>7</v>
+      </c>
+      <c r="B26" s="15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
+        <v>7</v>
+      </c>
+      <c r="B27" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
+        <v>8</v>
+      </c>
+      <c r="B28" s="15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>2</v>
+      </c>
+      <c r="B29" s="15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>4</v>
+      </c>
+      <c r="B30" s="15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
+        <v>0</v>
+      </c>
+      <c r="B31" s="15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
+        <v>8</v>
+      </c>
+      <c r="B32" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
+        <v>8</v>
+      </c>
+      <c r="B33" s="15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="14">
+        <v>6</v>
+      </c>
+      <c r="B34" s="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
+        <v>5</v>
+      </c>
+      <c r="B35" s="15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>0</v>
+      </c>
+      <c r="B36" s="15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
+        <v>1</v>
+      </c>
+      <c r="B37" s="15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="14">
+        <v>1</v>
+      </c>
+      <c r="B38" s="15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="14">
+        <v>13</v>
+      </c>
+      <c r="B39" s="15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="14">
+        <v>13</v>
+      </c>
+      <c r="B40" s="15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="14">
+        <v>13</v>
+      </c>
+      <c r="B41" s="15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="14">
+        <v>3</v>
+      </c>
+      <c r="B42" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="14">
+        <v>3</v>
+      </c>
+      <c r="B43" s="15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="14">
+        <v>8</v>
+      </c>
+      <c r="B44" s="15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="14">
+        <v>10</v>
+      </c>
+      <c r="B45" s="15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="14">
+        <v>10</v>
+      </c>
+      <c r="B46" s="15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="14">
+        <v>10</v>
+      </c>
+      <c r="B47" s="15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="14">
+        <v>4</v>
+      </c>
+      <c r="B48" s="15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="14">
+        <v>5</v>
+      </c>
+      <c r="B49" s="15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="14">
+        <v>5</v>
+      </c>
+      <c r="B50" s="15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="14">
+        <v>15</v>
+      </c>
+      <c r="B51" s="15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="14">
+        <v>5</v>
+      </c>
+      <c r="B52" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="14">
+        <v>1</v>
+      </c>
+      <c r="B53" s="15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="14">
+        <v>1</v>
+      </c>
+      <c r="B54" s="15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="14">
+        <v>4</v>
+      </c>
+      <c r="B55" s="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="14">
+        <v>1</v>
+      </c>
+      <c r="B56" s="15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="14">
+        <v>0</v>
+      </c>
+      <c r="B57" s="15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="14">
+        <v>10</v>
+      </c>
+      <c r="B58" s="15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="14">
+        <v>2</v>
+      </c>
+      <c r="B59" s="15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="14">
+        <v>8</v>
+      </c>
+      <c r="B60" s="15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="14">
+        <v>0</v>
+      </c>
+      <c r="B61" s="15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="14">
+        <v>5</v>
+      </c>
+      <c r="B62" s="15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="14">
+        <v>0</v>
+      </c>
+      <c r="B63" s="15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="14">
+        <v>8</v>
+      </c>
+      <c r="B64" s="15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="14">
+        <v>5</v>
+      </c>
+      <c r="B65" s="15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="14">
+        <v>10</v>
+      </c>
+      <c r="B66" s="15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="14">
+        <v>4</v>
+      </c>
+      <c r="B67" s="15">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="14">
+        <v>4</v>
+      </c>
+      <c r="B68" s="15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="14">
+        <v>1</v>
+      </c>
+      <c r="B69" s="15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="14">
+        <v>8</v>
+      </c>
+      <c r="B70" s="15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="14">
+        <v>8</v>
+      </c>
+      <c r="B71" s="15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="14">
+        <v>8</v>
+      </c>
+      <c r="B72" s="15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="14">
+        <v>0</v>
+      </c>
+      <c r="B73" s="15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="14">
+        <v>10</v>
+      </c>
+      <c r="B74" s="15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="18">
+        <v>8</v>
+      </c>
+      <c r="B75" s="19">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>